<commit_message>
feat: Fix google traslate
</commit_message>
<xml_diff>
--- a/MEMO.xlsx
+++ b/MEMO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otto\Desktop\ARCHIVOS A ENVIAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Manifiestos_NorOriente_Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8472" windowHeight="6888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8475" windowHeight="6885"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -581,19 +581,20 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
@@ -607,7 +608,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -617,8 +618,8 @@
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -638,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -646,7 +647,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -654,7 +655,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -662,7 +663,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -670,7 +671,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -678,7 +679,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -686,7 +687,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -694,7 +695,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -702,7 +703,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -710,7 +711,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -718,7 +719,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -726,7 +727,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -741,6 +742,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.51181102362204722" top="0.23622047244094491" bottom="0.15748031496062992" header="0.11811023622047245" footer="0.11811023622047245"/>
-  <pageSetup paperSize="345" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>